<commit_message>
add manual indent testing data
</commit_message>
<xml_diff>
--- a/Test Data/servo and indent testing.xlsx
+++ b/Test Data/servo and indent testing.xlsx
@@ -1,29 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mli138/workspace/Safe_Cracker/Test Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027092A3-E799-0A42-AD21-1F44A7072CE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E8CDB5-7CDF-4B49-AA16-34827503DEE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1600" windowWidth="29180" windowHeight="21880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14900" yWindow="4740" windowWidth="29180" windowHeight="21880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="servo calib1" sheetId="1" r:id="rId1"/>
     <sheet name="servo calib2" sheetId="2" r:id="rId2"/>
     <sheet name="indent tests" sheetId="3" r:id="rId3"/>
-    <sheet name="cracking3" sheetId="4" r:id="rId4"/>
+    <sheet name="Indent testing (Manual)" sheetId="5" r:id="rId4"/>
+    <sheet name="cracking3" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6802" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6834" uniqueCount="981">
   <si>
     <t>Dial stuck</t>
   </si>
@@ -2870,6 +2881,102 @@
   </si>
   <si>
     <t xml:space="preserve"> handlePosition</t>
+  </si>
+  <si>
+    <t>Indent Positions Manual Testing:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0: [97] 97 - </t>
+  </si>
+  <si>
+    <t>1: [6] 5 - 10?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2: [14] 14 - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3: [22] 22 - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4: [31] 31 - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5: [39] 39 - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6: [47] 48 - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7: [56] 56 - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8: [64] 64 - </t>
+  </si>
+  <si>
+    <t>9: [73] 72 - 74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10: [81] 80 - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11: [90] </t>
+  </si>
+  <si>
+    <t>hand measured</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t>chosen</t>
+  </si>
+  <si>
+    <t>difference</t>
+  </si>
+  <si>
+    <t>96 - 99</t>
+  </si>
+  <si>
+    <t>97 or 98</t>
+  </si>
+  <si>
+    <t>4 -8</t>
+  </si>
+  <si>
+    <t>12 - 16</t>
+  </si>
+  <si>
+    <t>21 - 25</t>
+  </si>
+  <si>
+    <t>29 - 33</t>
+  </si>
+  <si>
+    <t>37 - 42</t>
+  </si>
+  <si>
+    <t>39 or 40</t>
+  </si>
+  <si>
+    <t>45 - 50</t>
+  </si>
+  <si>
+    <t>47 or 48</t>
+  </si>
+  <si>
+    <t>54 - 58</t>
+  </si>
+  <si>
+    <t>63 - 67</t>
+  </si>
+  <si>
+    <t>71 - 75</t>
+  </si>
+  <si>
+    <t>79 - 83</t>
+  </si>
+  <si>
+    <t>88 - 92</t>
   </si>
 </sst>
 </file>
@@ -2891,12 +2998,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2926,7 +3039,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2934,6 +3047,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17129,7 +17244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1049"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -28229,7 +28344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -28690,6 +28805,283 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBA0C67-EC56-F24F-9A4D-EF37E162A9CB}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="B15" t="s">
+        <v>963</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>964</v>
+      </c>
+      <c r="D15" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="B16" t="s">
+        <v>967</v>
+      </c>
+      <c r="C16" s="4">
+        <v>98</v>
+      </c>
+      <c r="D16">
+        <f>C16-C27</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>968</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <f>100-C16+C17</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <f>C18-C17</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>970</v>
+      </c>
+      <c r="B19">
+        <v>23</v>
+      </c>
+      <c r="C19" s="4">
+        <v>23</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:D27" si="0">C19-C18</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>971</v>
+      </c>
+      <c r="B20">
+        <v>31</v>
+      </c>
+      <c r="C20" s="4">
+        <v>31</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>972</v>
+      </c>
+      <c r="B21" t="s">
+        <v>973</v>
+      </c>
+      <c r="C21" s="4">
+        <v>40</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>974</v>
+      </c>
+      <c r="B22" t="s">
+        <v>975</v>
+      </c>
+      <c r="C22" s="4">
+        <v>48</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="B23">
+        <v>56</v>
+      </c>
+      <c r="C23" s="4">
+        <v>56</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="B24">
+        <v>65</v>
+      </c>
+      <c r="C24" s="4">
+        <v>65</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>978</v>
+      </c>
+      <c r="B25">
+        <v>73</v>
+      </c>
+      <c r="C25" s="4">
+        <v>73</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="B26">
+        <v>81</v>
+      </c>
+      <c r="C26" s="4">
+        <v>81</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="B27">
+        <v>90</v>
+      </c>
+      <c r="C27" s="4">
+        <v>90</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I939"/>
   <sheetViews>

</xml_diff>